<commit_message>
digitalized table nfishers 36-38. Incorporating these years into processed table. Fixing discrepancy for year 1935
</commit_message>
<xml_diff>
--- a/data/landings/cdfw/public/fish_bulletins/raw/fb49/raw/Table144.xlsx
+++ b/data/landings/cdfw/public/fish_bulletins/raw/fb49/raw/Table144.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/camilavargaspoulsen/github/wc_climate_synthesis/data/landings/cdfw/public/fish_bulletins/raw/fb49/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D937844B-44A5-244B-8C2B-AB01B5FBBB19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{583990CD-B846-C540-B3E6-B5C6D8DB0F8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="12800" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="27">
   <si>
     <r>
       <rPr>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Others</t>
   </si>
 </sst>
 </file>
@@ -165,13 +168,19 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="15">
     <border>
@@ -283,7 +292,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -334,6 +343,12 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -648,17 +663,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="30"/>
-    <col min="2" max="2" width="55"/>
-    <col min="3" max="3" width="31"/>
+    <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.15">
@@ -1027,6 +1042,17 @@
         <v>12</v>
       </c>
     </row>
+    <row r="34" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+      <c r="A34" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34" s="21">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>